<commit_message>
IWEREYOU-44 Create function point files
</commit_message>
<xml_diff>
--- a/Doc/FunctionPoints/FP_Chart_new.xlsx
+++ b/Doc/FunctionPoints/FP_Chart_new.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Login</t>
   </si>
@@ -39,6 +39,30 @@
   </si>
   <si>
     <t>Hours</t>
+  </si>
+  <si>
+    <t>Invite a friend</t>
+  </si>
+  <si>
+    <t>View/ Update Profile</t>
+  </si>
+  <si>
+    <t>Manage Challenges</t>
+  </si>
+  <si>
+    <t>Answer Challenge</t>
+  </si>
+  <si>
+    <t>Manage Contacts (Create/ Show)</t>
+  </si>
+  <si>
+    <t>Delete Contact</t>
+  </si>
+  <si>
+    <t>Calculated Hours</t>
+  </si>
+  <si>
+    <t>Registration + Login</t>
   </si>
 </sst>
 </file>
@@ -109,13 +133,23 @@
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="6.2720589245715996E-2"/>
+          <c:y val="0.16203703703703703"/>
+          <c:w val="0.86681984123712286"/>
+          <c:h val="0.74915135608048999"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="0"/>
           <c:tx>
             <c:strRef>
               <c:f>Sheet1!$C$1</c:f>
@@ -306,6 +340,38 @@
                 </c:ext>
               </c:extLst>
             </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>Manage</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t> Contacts</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -345,6 +411,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -379,36 +446,42 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$4</c:f>
+              <c:f>Sheet1!$D$2:$D$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.5</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$4</c:f>
+              <c:f>Sheet1!$C$2:$C$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>15.8</c:v>
+                  <c:v>33.15</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25.28</c:v>
+                  <c:v>51.85</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18.170000000000002</c:v>
+                  <c:v>28.05</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>35.700000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -423,14 +496,14 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="237425872"/>
-        <c:axId val="237427832"/>
+        <c:axId val="323755304"/>
+        <c:axId val="323753736"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
               <c15:ser>
                 <c:idx val="0"/>
-                <c:order val="0"/>
+                <c:order val="1"/>
                 <c:spPr>
                   <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
                     <a:noFill/>
@@ -493,13 +566,13 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="3"/>
                       <c:pt idx="0">
-                        <c:v>15.8</c:v>
+                        <c:v>33.15</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>25.28</c:v>
+                        <c:v>51.85</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>18.170000000000002</c:v>
+                        <c:v>28.05</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -520,7 +593,7 @@
                         <c:v>1.5</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>4.5</c:v>
+                        <c:v>8</c:v>
                       </c:pt>
                       <c:pt idx="2">
                         <c:v>1.5</c:v>
@@ -535,7 +608,7 @@
         </c:extLst>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="237425872"/>
+        <c:axId val="323755304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -628,12 +701,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="237427832"/>
+        <c:crossAx val="323753736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="237427832"/>
+        <c:axId val="323753736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -727,7 +800,698 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="237425872"/>
+        <c:crossAx val="323755304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:alpha val="0"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="6.2720589245715996E-2"/>
+          <c:y val="0.16203703703703703"/>
+          <c:w val="0.86681984123712286"/>
+          <c:h val="0.74915135608048999"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Function Points</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+              <a:noFill/>
+              <a:prstDash val="sysDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{AF0B3B22-5194-44E6-A6DE-2A60B14974C9}" type="CELLREF">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLREF]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="de-DE"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable>
+                    <c15:dlblFTEntry>
+                      <c15:txfldGUID>{AF0B3B22-5194-44E6-A6DE-2A60B14974C9}</c15:txfldGUID>
+                      <c15:f>Sheet1!$B$4</c15:f>
+                      <c15:dlblFieldTableCache>
+                        <c:ptCount val="1"/>
+                        <c:pt idx="0">
+                          <c:v>Delete Account</c:v>
+                        </c:pt>
+                      </c15:dlblFieldTableCache>
+                    </c15:dlblFTEntry>
+                  </c15:dlblFieldTable>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>Manage</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t> Contacts</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>Register + Login</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="rnd">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.26435156079798328"/>
+                  <c:y val="5.0925925925925923E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$4:$D$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$4:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>28.05</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>35.700000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>85</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="326241848"/>
+        <c:axId val="326240672"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="1"/>
+                <c:spPr>
+                  <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+                    <a:noFill/>
+                    <a:prstDash val="sysDot"/>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:gradFill rotWithShape="1">
+                      <a:gsLst>
+                        <a:gs pos="0">
+                          <a:schemeClr val="accent1">
+                            <a:lumMod val="110000"/>
+                            <a:satMod val="105000"/>
+                            <a:tint val="67000"/>
+                          </a:schemeClr>
+                        </a:gs>
+                        <a:gs pos="50000">
+                          <a:schemeClr val="accent1">
+                            <a:lumMod val="105000"/>
+                            <a:satMod val="103000"/>
+                            <a:tint val="73000"/>
+                          </a:schemeClr>
+                        </a:gs>
+                        <a:gs pos="100000">
+                          <a:schemeClr val="accent1">
+                            <a:lumMod val="105000"/>
+                            <a:satMod val="109000"/>
+                            <a:tint val="81000"/>
+                          </a:schemeClr>
+                        </a:gs>
+                      </a:gsLst>
+                      <a:lin ang="5400000" scaled="0"/>
+                    </a:gradFill>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1">
+                          <a:shade val="95000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$C$2:$C$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="3"/>
+                      <c:pt idx="0">
+                        <c:v>33.15</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>51.85</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>28.05</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$D$2:$D$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="3"/>
+                      <c:pt idx="0">
+                        <c:v>1.5</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>1.5</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+          </c:ext>
+        </c:extLst>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="326241848"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Hours</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="20000"/>
+                <a:lumOff val="80000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="326240672"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="326240672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Function Points</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="326241848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -794,16 +1558,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -817,6 +1581,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1088,16 +1884,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D4"/>
+  <dimension ref="B1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:4" x14ac:dyDescent="0.25">
@@ -1113,7 +1910,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>15.8</v>
+        <v>33.15</v>
       </c>
       <c r="D2">
         <v>1.5</v>
@@ -1124,10 +1921,10 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>25.28</v>
+        <v>51.85</v>
       </c>
       <c r="D3">
-        <v>4.5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
@@ -1135,10 +1932,99 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>18.170000000000002</v>
+        <v>28.05</v>
       </c>
       <c r="D4">
         <v>1.5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>35.700000000000003</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <f>SUM(C2:C3)</f>
+        <v>85</v>
+      </c>
+      <c r="D6">
+        <f>SUM(D2:D3)</f>
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>28.05</v>
+      </c>
+      <c r="D8">
+        <f t="shared" ref="D8:D10" si="0">(C8-10.662)/7.2977</f>
+        <v>2.3826685119969304</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>47.6</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>5.0615947490305171</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10">
+        <v>36.549999999999997</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>3.5474190498376199</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11">
+        <v>44.2</v>
+      </c>
+      <c r="D11">
+        <f>(C11-10.662)/7.2977</f>
+        <v>4.5956945338942417</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>41.65</v>
+      </c>
+      <c r="D12">
+        <f>(C12-10.662)/7.2977</f>
+        <v>4.2462693725420335</v>
       </c>
     </row>
   </sheetData>

</xml_diff>